<commit_message>
- Correction dans le fichier d'inscriptions.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21016 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/inscriptions-web.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/inscriptions-web.xlsx
@@ -13936,8 +13936,8 @@
   <dimension ref="A1:J1990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <pane ySplit="1" topLeftCell="A628" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D689" sqref="D689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31225,11 +31225,11 @@
       <c r="A690" s="3">
         <v>41265.535879629599</v>
       </c>
-      <c r="B690" s="2"/>
+      <c r="B690" s="2" t="s">
+        <v>1891</v>
+      </c>
       <c r="C690" s="2"/>
-      <c r="D690" s="2" t="s">
-        <v>1891</v>
-      </c>
+      <c r="D690" s="2"/>
       <c r="E690" s="2"/>
       <c r="F690" s="2" t="s">
         <v>1892</v>

</xml_diff>

<commit_message>
- Rajouté quelques lignes dans le fichier d'inscriptions.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@21028 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/inscriptions-web.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Bonne nouvelle/inscriptions-web.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11736" uniqueCount="5199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11837" uniqueCount="5252">
   <si>
     <t>Horodateur</t>
   </si>
@@ -15614,6 +15614,165 @@
   </si>
   <si>
     <t>Av. du Tirage 5</t>
+  </si>
+  <si>
+    <t>Roth Durr</t>
+  </si>
+  <si>
+    <t>Scheibler</t>
+  </si>
+  <si>
+    <t>Chaignat</t>
+  </si>
+  <si>
+    <t>Schneller</t>
+  </si>
+  <si>
+    <t>Derron-Notter</t>
+  </si>
+  <si>
+    <t>Chadourne</t>
+  </si>
+  <si>
+    <t>Jaccard Krejci</t>
+  </si>
+  <si>
+    <t>Stähli</t>
+  </si>
+  <si>
+    <t>Fillon Marguerat</t>
+  </si>
+  <si>
+    <t>Felix</t>
+  </si>
+  <si>
+    <t>Wittwer</t>
+  </si>
+  <si>
+    <t>Schär-Rossier</t>
+  </si>
+  <si>
+    <t>Parisod-Gorjat</t>
+  </si>
+  <si>
+    <t>Marc et Marlyse</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Chalet le Torrent</t>
+  </si>
+  <si>
+    <t>Rütiwaldstrasse 18</t>
+  </si>
+  <si>
+    <t>route du Chaussié 3</t>
+  </si>
+  <si>
+    <t>Pra Pury 20</t>
+  </si>
+  <si>
+    <t>Meylandstrasse 14</t>
+  </si>
+  <si>
+    <t>CP 3106</t>
+  </si>
+  <si>
+    <t>avenue du Bois-de-la-Chapelle 79</t>
+  </si>
+  <si>
+    <t>Au Village 36</t>
+  </si>
+  <si>
+    <t>rue Jean-Violette 12</t>
+  </si>
+  <si>
+    <t>impasse des Chaffeirus  19</t>
+  </si>
+  <si>
+    <t>au Village 13</t>
+  </si>
+  <si>
+    <t>route du Marchet 15</t>
+  </si>
+  <si>
+    <t>route de l'Aclex 1</t>
+  </si>
+  <si>
+    <t>route de la Gare 41</t>
+  </si>
+  <si>
+    <t>avenue A.-F.-Dubois 58</t>
+  </si>
+  <si>
+    <t>L'Essert 11</t>
+  </si>
+  <si>
+    <t>route de Riaz 2</t>
+  </si>
+  <si>
+    <t>Home du Vully - route de la Gare 12</t>
+  </si>
+  <si>
+    <t>Herisau</t>
+  </si>
+  <si>
+    <t>Vuisternens-devant-Romont</t>
+  </si>
+  <si>
+    <t>Morat</t>
+  </si>
+  <si>
+    <t>Neuchâtel</t>
+  </si>
+  <si>
+    <t>Onex</t>
+  </si>
+  <si>
+    <t>Sugiez</t>
+  </si>
+  <si>
+    <t>Surpierre</t>
+  </si>
+  <si>
+    <t>Genève</t>
+  </si>
+  <si>
+    <t>Châtonnaye</t>
+  </si>
+  <si>
+    <t>Neyruz</t>
+  </si>
+  <si>
+    <t>Nuvilly</t>
+  </si>
+  <si>
+    <t>Estavayer-le-Lac</t>
+  </si>
+  <si>
+    <t>Meyrin</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Middes</t>
+  </si>
+  <si>
+    <t>Bulle</t>
+  </si>
+  <si>
+    <t>Rte des Baumes 2</t>
+  </si>
+  <si>
+    <t>Zürichbergstrasse 136</t>
+  </si>
+  <si>
+    <t>Région</t>
   </si>
 </sst>
 </file>
@@ -15623,11 +15782,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -15691,15 +15857,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -15708,15 +15875,30 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -16015,11 +16197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2351"/>
+  <dimension ref="A1:K2372"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2267" sqref="C2267"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16033,7 +16215,7 @@
     <col min="9" max="9" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16064,8 +16246,11 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>5251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>41137.487604166701</v>
       </c>
@@ -16090,7 +16275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>41139.531643518501</v>
       </c>
@@ -16115,7 +16300,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>41150.4466203704</v>
       </c>
@@ -16140,7 +16325,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>41150.640659722201</v>
       </c>
@@ -16165,7 +16350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>41151.353078703702</v>
       </c>
@@ -16190,7 +16375,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>41151.416956018496</v>
       </c>
@@ -16215,7 +16400,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>41151.711979166699</v>
       </c>
@@ -16240,7 +16425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>41151.846539351798</v>
       </c>
@@ -16265,7 +16450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>41152.293460648201</v>
       </c>
@@ -16292,7 +16477,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>41152.339305555601</v>
       </c>
@@ -16317,7 +16502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>41152.381111111099</v>
       </c>
@@ -16342,7 +16527,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>41152.425104166701</v>
       </c>
@@ -16367,7 +16552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>41152.429710648103</v>
       </c>
@@ -16392,7 +16577,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>41152.448553240698</v>
       </c>
@@ -16417,7 +16602,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>41152.457696759302</v>
       </c>
@@ -73510,6 +73695,466 @@
         <v>737</v>
       </c>
     </row>
+    <row r="2353" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2353" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2353" s="8" t="s">
+        <v>5199</v>
+      </c>
+      <c r="E2353" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="F2353" s="10" t="s">
+        <v>5215</v>
+      </c>
+      <c r="H2353" s="12">
+        <v>3961</v>
+      </c>
+      <c r="I2353" s="11" t="s">
+        <v>1584</v>
+      </c>
+      <c r="K2353" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2354" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2354" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2354" s="8" t="s">
+        <v>5200</v>
+      </c>
+      <c r="E2354" s="9" t="s">
+        <v>4576</v>
+      </c>
+      <c r="F2354" s="10" t="s">
+        <v>5216</v>
+      </c>
+      <c r="H2354" s="12">
+        <v>9100</v>
+      </c>
+      <c r="I2354" s="11" t="s">
+        <v>5233</v>
+      </c>
+      <c r="K2354" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2355" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2355" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2355" s="8" t="s">
+        <v>3200</v>
+      </c>
+      <c r="E2355" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="F2355" s="10" t="s">
+        <v>5217</v>
+      </c>
+      <c r="H2355" s="14">
+        <v>1687</v>
+      </c>
+      <c r="I2355" s="13" t="s">
+        <v>5234</v>
+      </c>
+      <c r="K2355" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2356" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2356" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2356" s="8" t="s">
+        <v>2783</v>
+      </c>
+      <c r="E2356" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="F2356" s="10" t="s">
+        <v>5218</v>
+      </c>
+      <c r="H2356" s="12">
+        <v>3280</v>
+      </c>
+      <c r="I2356" s="11" t="s">
+        <v>5235</v>
+      </c>
+      <c r="K2356" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2357" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2357" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2357" s="8" t="s">
+        <v>5201</v>
+      </c>
+      <c r="E2357" s="9" t="s">
+        <v>909</v>
+      </c>
+      <c r="F2357" s="10" t="s">
+        <v>5219</v>
+      </c>
+      <c r="H2357" s="12">
+        <v>3280</v>
+      </c>
+      <c r="I2357" s="11" t="s">
+        <v>5235</v>
+      </c>
+      <c r="K2357" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2358" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2358" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2358" s="8" t="s">
+        <v>5202</v>
+      </c>
+      <c r="E2358" s="9" t="s">
+        <v>1904</v>
+      </c>
+      <c r="G2358" s="10" t="s">
+        <v>5220</v>
+      </c>
+      <c r="H2358" s="12">
+        <v>2001</v>
+      </c>
+      <c r="I2358" s="11" t="s">
+        <v>5236</v>
+      </c>
+      <c r="K2358" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2359" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2359" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D2359" s="8" t="s">
+        <v>5108</v>
+      </c>
+      <c r="E2359" s="9" t="s">
+        <v>5212</v>
+      </c>
+      <c r="F2359" s="10" t="s">
+        <v>5221</v>
+      </c>
+      <c r="H2359" s="12">
+        <v>1213</v>
+      </c>
+      <c r="I2359" s="11" t="s">
+        <v>5237</v>
+      </c>
+      <c r="K2359" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2360" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2360" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2360" s="8" t="s">
+        <v>5203</v>
+      </c>
+      <c r="E2360" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="F2360" s="10" t="s">
+        <v>5249</v>
+      </c>
+      <c r="H2360" s="12">
+        <v>1786</v>
+      </c>
+      <c r="I2360" s="11" t="s">
+        <v>5238</v>
+      </c>
+      <c r="K2360" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2361" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2361" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2361" s="8" t="s">
+        <v>2371</v>
+      </c>
+      <c r="E2361" s="9" t="s">
+        <v>883</v>
+      </c>
+      <c r="F2361" s="10" t="s">
+        <v>5222</v>
+      </c>
+      <c r="H2361" s="12">
+        <v>1528</v>
+      </c>
+      <c r="I2361" s="11" t="s">
+        <v>5239</v>
+      </c>
+      <c r="K2361" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2362" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2362" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2362" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E2362" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="F2362" s="10" t="s">
+        <v>5223</v>
+      </c>
+      <c r="H2362" s="12">
+        <v>1205</v>
+      </c>
+      <c r="I2362" s="11" t="s">
+        <v>5240</v>
+      </c>
+      <c r="K2362" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2363" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2363" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2363" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="E2363" s="9" t="s">
+        <v>1904</v>
+      </c>
+      <c r="F2363" s="10" t="s">
+        <v>5224</v>
+      </c>
+      <c r="H2363" s="12">
+        <v>1553</v>
+      </c>
+      <c r="I2363" s="13" t="s">
+        <v>5241</v>
+      </c>
+      <c r="K2363" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2364" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2364" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2364" s="8" t="s">
+        <v>5204</v>
+      </c>
+      <c r="E2364" s="9" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F2364" s="10" t="s">
+        <v>5225</v>
+      </c>
+      <c r="H2364" s="12">
+        <v>1483</v>
+      </c>
+      <c r="I2364" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="K2364" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2365" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2365" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2365" s="8" t="s">
+        <v>5205</v>
+      </c>
+      <c r="E2365" s="9" t="s">
+        <v>2735</v>
+      </c>
+      <c r="F2365" s="10" t="s">
+        <v>5226</v>
+      </c>
+      <c r="H2365" s="12">
+        <v>1740</v>
+      </c>
+      <c r="I2365" s="11" t="s">
+        <v>5242</v>
+      </c>
+      <c r="K2365" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2366" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2366" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2366" s="8" t="s">
+        <v>5206</v>
+      </c>
+      <c r="E2366" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2366" s="10" t="s">
+        <v>5227</v>
+      </c>
+      <c r="H2366" s="12">
+        <v>1485</v>
+      </c>
+      <c r="I2366" s="11" t="s">
+        <v>5243</v>
+      </c>
+      <c r="K2366" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2367" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2367" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2367" s="8" t="s">
+        <v>5207</v>
+      </c>
+      <c r="E2367" s="9" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F2367" s="10" t="s">
+        <v>5228</v>
+      </c>
+      <c r="H2367" s="12">
+        <v>1470</v>
+      </c>
+      <c r="I2367" s="13" t="s">
+        <v>5244</v>
+      </c>
+      <c r="K2367" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2368" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2368" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2368" s="8" t="s">
+        <v>5208</v>
+      </c>
+      <c r="E2368" s="9" t="s">
+        <v>5213</v>
+      </c>
+      <c r="F2368" s="10" t="s">
+        <v>5229</v>
+      </c>
+      <c r="H2368" s="12">
+        <v>1217</v>
+      </c>
+      <c r="I2368" s="11" t="s">
+        <v>5245</v>
+      </c>
+      <c r="K2368" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2369" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2369" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2369" s="8" t="s">
+        <v>5209</v>
+      </c>
+      <c r="E2369" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="F2369" s="10" t="s">
+        <v>5250</v>
+      </c>
+      <c r="H2369" s="12">
+        <v>8044</v>
+      </c>
+      <c r="I2369" s="11" t="s">
+        <v>5246</v>
+      </c>
+      <c r="K2369" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2370" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2370" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2370" s="8" t="s">
+        <v>5210</v>
+      </c>
+      <c r="E2370" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2370" s="10" t="s">
+        <v>5230</v>
+      </c>
+      <c r="H2370" s="12">
+        <v>1749</v>
+      </c>
+      <c r="I2370" s="11" t="s">
+        <v>5247</v>
+      </c>
+      <c r="K2370" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2371" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2371" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2371" s="8" t="s">
+        <v>1529</v>
+      </c>
+      <c r="E2371" s="9" t="s">
+        <v>5214</v>
+      </c>
+      <c r="F2371" s="10" t="s">
+        <v>5231</v>
+      </c>
+      <c r="H2371" s="12">
+        <v>1630</v>
+      </c>
+      <c r="I2371" s="11" t="s">
+        <v>5248</v>
+      </c>
+      <c r="K2371" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2372" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2372" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2372" s="8" t="s">
+        <v>5211</v>
+      </c>
+      <c r="E2372" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2372" s="10" t="s">
+        <v>5232</v>
+      </c>
+      <c r="H2372" s="12">
+        <v>1786</v>
+      </c>
+      <c r="I2372" s="11" t="s">
+        <v>5238</v>
+      </c>
+      <c r="K2372" s="12">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>